<commit_message>
updated webapp using env
</commit_message>
<xml_diff>
--- a/data/chu2016_dataentry.xlsx
+++ b/data/chu2016_dataentry.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alpha Tauri\Dropbox (GaTech)\Aaron and Rahul Shared Files\ofet-db\mongodb_v2022\P3HT\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\GitHub\ofet-db\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDD8A1B-E91E-4129-8B31-620FBB776F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BFCDD9-BAA4-4AC1-9BC7-4C040A8FE87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F9416C1E-603F-4BBF-9408-B5C89C02A1C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F9416C1E-603F-4BBF-9408-B5C89C02A1C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -662,13 +662,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CA63BF-5294-4760-AB4B-083BE97F71AD}">
   <dimension ref="A1:AW11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -1896,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83375AC-B1F1-40C0-BC38-F9FB51C023BC}">
   <dimension ref="A1:A49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>